<commit_message>
feat: enhance participant mapping and additional variables handling in converter UI
</commit_message>
<xml_diff>
--- a/examples/workshop/exercise_1_raw_data/raw_data/wellbeing.xlsx
+++ b/examples/workshop/exercise_1_raw_data/raw_data/wellbeing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10222"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karl/work/github/psycho-validator/examples/workshop/exercise_1_raw_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A13E3A08-0725-274A-86A5-ABC6E79CADCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9C4824-CCBB-0B48-B112-43F00496ECEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="2220" windowWidth="28240" windowHeight="17240" xr2:uid="{2ED3946B-4463-9B48-BB4A-E5571941758E}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>participant_id</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>DEMO020</t>
+  </si>
+  <si>
+    <t>sleep</t>
   </si>
 </sst>
 </file>
@@ -986,15 +989,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75CA3F8-C212-794B-9380-2C703DEB7DBD}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="19.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1031,8 +1037,11 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1069,8 +1078,11 @@
       <c r="L2" s="1">
         <v>45672</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1107,8 +1119,11 @@
       <c r="L3" s="1">
         <v>45673</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1145,8 +1160,11 @@
       <c r="L4" s="1">
         <v>45674</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1183,8 +1201,11 @@
       <c r="L5" s="1">
         <v>45675</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1221,8 +1242,11 @@
       <c r="L6" s="1">
         <v>45676</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1259,8 +1283,11 @@
       <c r="L7" s="1">
         <v>45677</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1297,8 +1324,11 @@
       <c r="L8" s="1">
         <v>45678</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1335,8 +1365,11 @@
       <c r="L9" s="1">
         <v>45679</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1373,8 +1406,11 @@
       <c r="L10" s="1">
         <v>45680</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1411,8 +1447,11 @@
       <c r="L11" s="1">
         <v>45681</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1449,8 +1488,11 @@
       <c r="L12" s="1">
         <v>45672</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1487,8 +1529,11 @@
       <c r="L13" s="1">
         <v>45673</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1525,8 +1570,11 @@
       <c r="L14" s="1">
         <v>45674</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1563,8 +1611,11 @@
       <c r="L15" s="1">
         <v>45675</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1601,8 +1652,11 @@
       <c r="L16" s="1">
         <v>45676</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1639,8 +1693,11 @@
       <c r="L17" s="1">
         <v>45677</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1677,8 +1734,11 @@
       <c r="L18" s="1">
         <v>45678</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1715,8 +1775,11 @@
       <c r="L19" s="1">
         <v>45679</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1753,8 +1816,11 @@
       <c r="L20" s="1">
         <v>45680</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1790,6 +1856,9 @@
       </c>
       <c r="L21" s="1">
         <v>45681</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>